<commit_message>
update on ahp algo
1. file transfer,
2. eigen value
</commit_message>
<xml_diff>
--- a/SummaryAhpScale.xlsx
+++ b/SummaryAhpScale.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Kerja Sawada Offline\Shiny R Tutorial\AHP in R\AHP trial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6B65A8E-61D7-45C7-ABA5-FE5634D3B4CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E929C534-9618-4512-BC4C-E7AB745C9683}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{6BF63009-C8D4-493E-897C-B3ABD3122CEF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{6BF63009-C8D4-493E-897C-B3ABD3122CEF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Level1" sheetId="1" r:id="rId1"/>
-    <sheet name="Level2_Econ" sheetId="2" r:id="rId2"/>
+    <sheet name="Level2_Econ" sheetId="2" r:id="rId1"/>
+    <sheet name="Level1" sheetId="6" r:id="rId2"/>
     <sheet name="Level2_Technical" sheetId="3" r:id="rId3"/>
     <sheet name="Level2_Infrastructure" sheetId="4" r:id="rId4"/>
     <sheet name="Level2_serviceStandard" sheetId="5" r:id="rId5"/>
@@ -38,28 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Technical_Economic</t>
-  </si>
-  <si>
-    <t>Technical_Infrastructure</t>
-  </si>
-  <si>
-    <t>Economic_Infrastructure</t>
-  </si>
-  <si>
-    <t>Economic_serviceStandard</t>
-  </si>
-  <si>
-    <t>Infrastructure_serviceStandard</t>
-  </si>
-  <si>
-    <t>Technical_serviceStandard</t>
-  </si>
-  <si>
-    <t>`</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Capex_Opex</t>
   </si>
@@ -104,6 +83,24 @@
   </si>
   <si>
     <t>Freq_Scalibility</t>
+  </si>
+  <si>
+    <t>Tech_Econ</t>
+  </si>
+  <si>
+    <t>Tech_Infra</t>
+  </si>
+  <si>
+    <t>Tech_serviceStandard</t>
+  </si>
+  <si>
+    <t>Econ_Infra</t>
+  </si>
+  <si>
+    <t>Econ_serviceStandard</t>
+  </si>
+  <si>
+    <t>Infra_serviceStandard</t>
   </si>
 </sst>
 </file>
@@ -544,74 +541,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21F4B89-79E5-4044-BAD8-CC0DC6D59C20}">
-  <dimension ref="A1:F10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>-3</v>
-      </c>
-      <c r="F2">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117F2B6E-6F6E-4C9C-A81D-1E16871FA296}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -623,7 +552,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -636,11 +565,66 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94E5D4C-1479-41A5-835F-69CD4EC30962}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>-3</v>
+      </c>
+      <c r="F2">
+        <v>-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7064BE98-FF21-4428-BF1F-8B115C4D7DDE}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -648,34 +632,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -727,7 +711,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -752,13 +736,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
need solution for <3 criteria
problem 1. AHP Cannot work on less than 3 criteria
error = "Number of observations censored = 1"
Error in array(x, c(length(x), 1L), if (!is.null(names(x))) list(names(x),  :
  'data' must be of a vector type, was 'NULL'
</commit_message>
<xml_diff>
--- a/SummaryAhpScale.xlsx
+++ b/SummaryAhpScale.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Kerja Sawada Offline\Shiny R Tutorial\AHP in R\AHP trial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E929C534-9618-4512-BC4C-E7AB745C9683}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614A5F1F-2850-4E00-B82D-19D7BC406C1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{6BF63009-C8D4-493E-897C-B3ABD3122CEF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Level2_Econ" sheetId="2" r:id="rId1"/>
-    <sheet name="Level1" sheetId="6" r:id="rId2"/>
-    <sheet name="Level2_Technical" sheetId="3" r:id="rId3"/>
-    <sheet name="Level2_Infrastructure" sheetId="4" r:id="rId4"/>
-    <sheet name="Level2_serviceStandard" sheetId="5" r:id="rId5"/>
+    <sheet name="Level2_EconTest" sheetId="2" r:id="rId1"/>
+    <sheet name="Level2_Econ" sheetId="7" r:id="rId2"/>
+    <sheet name="Level1" sheetId="6" r:id="rId3"/>
+    <sheet name="Level2_Technical" sheetId="3" r:id="rId4"/>
+    <sheet name="Level2_Infrastructure" sheetId="4" r:id="rId5"/>
+    <sheet name="Level2_serviceStandard" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Capex_Opex</t>
   </si>
@@ -101,6 +102,9 @@
   </si>
   <si>
     <t>Infra_serviceStandard</t>
+  </si>
+  <si>
+    <t>empty</t>
   </si>
 </sst>
 </file>
@@ -542,11 +546,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117F2B6E-6F6E-4C9C-A81D-1E16871FA296}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5C8A83-15AA-4EE7-BA0E-C6BC75A43188}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -565,11 +604,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94E5D4C-1479-41A5-835F-69CD4EC30962}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -620,12 +659,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7064BE98-FF21-4428-BF1F-8B115C4D7DDE}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,7 +738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A79764C-996A-4805-9A58-75D2FB63972D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -724,7 +763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B053AF8E-34B5-412F-B325-C941F89296DA}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
fail for <3 criteria
problem 1. Cannot work on less than 3 criteria
[1] "Number of observations censored = 1"
Error in array(x, c(length(x), 1L), if (!is.null(names(x))) list(names(x),  :
  'data' must be of a vector type, was 'NULL'
</commit_message>
<xml_diff>
--- a/SummaryAhpScale.xlsx
+++ b/SummaryAhpScale.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Kerja Sawada Offline\Shiny R Tutorial\AHP in R\AHP trial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614A5F1F-2850-4E00-B82D-19D7BC406C1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C751BF-4008-4C2C-BE8A-0B0328C2BF7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{6BF63009-C8D4-493E-897C-B3ABD3122CEF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{6BF63009-C8D4-493E-897C-B3ABD3122CEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Level2_EconTest" sheetId="2" r:id="rId1"/>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117F2B6E-6F6E-4C9C-A81D-1E16871FA296}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,10 +570,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5C8A83-15AA-4EE7-BA0E-C6BC75A43188}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>